<commit_message>
Atualização automática de ANTONIO_PRADO.xlsx
</commit_message>
<xml_diff>
--- a/ANTONIO_PRADO.xlsx
+++ b/ANTONIO_PRADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C360FF1B-C60A-48B9-9810-524961FE753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A45190-4230-4C64-8975-D85F50BEF82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1074,7 +1061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1134,36 +1121,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1202,14 +1165,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1256,7 +1214,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{F4AB0682-BDD5-4AC6-AA43-AAA15C639EE9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2ED0DFC3-F92B-45F0-872E-513398F8E7D1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1286,10 +1244,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27318111-05EC-4F00-BC80-7C62AD808966}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6F898A9-8796-4553-846D-EEF60ED9621D}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1327,7 +1285,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FDCC06F-CFD2-4B38-B2B9-64FAE1003AF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D7903B-CF51-44E6-B774-AE16A60BDB8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1390,7 +1348,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B9289EB-9B3B-42A1-ACB4-C9861AF6244C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{416408FE-9530-4841-A2DF-6C18D93FBEFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1409,7 +1367,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A94D1FFC-E67D-86ED-1FA5-268012B7D62B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C57659EB-7993-41A5-A2F5-658C8BA51741}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1458,7 +1416,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7897BAD-91D5-4055-8E72-BA218EE5D851}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C1F2EDF-34DE-A018-356F-4F41BE0F8DB2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1477,7 +1435,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80869E83-5D3C-D329-EB27-EA605F0B8F3C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A6309B-8401-B5B2-8921-19504CECB1A8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1508,7 +1466,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26B639F6-78C4-EF28-DDD2-FD4A4D16B218}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A802783-1753-CA30-4E08-DA80CD6B5979}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1539,7 +1497,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{781D0F48-580D-3133-1472-C33BF41C76DA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6492B70-C79F-99B7-D83D-4F5995531B9E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1582,7 +1540,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9799F407-A1E4-4AB8-9045-0326AADD2559}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6804F83-3579-4D57-B2AD-BCDFFAB9FB6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1620,7 +1578,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36C8B2ED-05F1-461D-B3FD-FED967A59185}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04990CD7-0DFD-4AC3-A56E-7488871B6643}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1663,7 +1621,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F97BF0F-7F05-493B-86F5-48B454AE2392}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C37BF8-9051-4A96-B853-26A52BC31822}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E7DBDA-D86A-48D5-A67E-69962E1676D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C17EC5-9253-4AB9-AB13-964462ADDA30}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1988,98 +1946,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="38"/>
-    <col min="6" max="6" width="2" style="38" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="38"/>
+    <col min="1" max="5" width="12.5703125" style="35"/>
+    <col min="6" max="6" width="2" style="35" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="37"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="37"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="37"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="37"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="37"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="37"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="37"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="37"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="37"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="37"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="37"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="37"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="37"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="37"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="37"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="37"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="37"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="37"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="37"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="37"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="37"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="37"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="37"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="37"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="37"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="37"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="37"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="37"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="37"/>
+      <c r="F29" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5341,19 +5299,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5376,57 +5334,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>271</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>271</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5451,54 +5409,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="21" t="s">
         <v>294</v>
       </c>
     </row>
@@ -5509,43 +5468,43 @@
       <c r="B2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="24">
         <v>45170</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="25">
         <v>1568</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="26">
         <v>4053</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="26">
         <v>627</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="27" t="s">
         <v>297</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="28" t="s">
         <v>299</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="28" t="s">
         <v>299</v>
       </c>
     </row>
@@ -5576,25 +5535,24 @@
       <c r="B1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="E1" s="33">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="30">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="33">
         <v>41</v>
       </c>
-      <c r="F1" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>302</v>
-      </c>
-      <c r="B2" s="36">
-        <v>41</v>
-      </c>
-      <c r="C2" s="34">
+      <c r="C2" s="31">
         <v>2.711281576511044E-3</v>
       </c>
     </row>

</xml_diff>